<commit_message>
updated adult subject log and started pilot data analysis
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/elizabeth_adult_subject_log.xlsx
+++ b/data/01_participant_logs/elizabeth_adult_subject_log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC_NOVEL/adult_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BC8784-5126-5940-9AB5-F652925AFF1E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBCB0D7-4DD5-A842-8B21-E571B6E8AF39}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{7F77447E-73EC-4A43-A6DE-AF98E6954F7E}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{7F77447E-73EC-4A43-A6DE-AF98E6954F7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
   <si>
     <t>ES</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>NF</t>
+  </si>
+  <si>
+    <t>SAN-080318-02</t>
   </si>
 </sst>
 </file>
@@ -627,7 +633,7 @@
   <dimension ref="A1:O128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,16 +1217,30 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43315</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>

</xml_diff>

<commit_message>
updated adult subject log 8/10/18
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/elizabeth_adult_subject_log.xlsx
+++ b/data/01_participant_logs/elizabeth_adult_subject_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBCB0D7-4DD5-A842-8B21-E571B6E8AF39}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE92C92-D0FD-9041-A51E-F847CFB4CF4D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{7F77447E-73EC-4A43-A6DE-AF98E6954F7E}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="77">
   <si>
     <t>ES</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>pilot A</t>
   </si>
   <si>
@@ -232,6 +229,33 @@
   </si>
   <si>
     <t>SAN-080318-02</t>
+  </si>
+  <si>
+    <t>SAN-080618-01</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>Wore glasses but eye tracker seemed mostly fine</t>
+  </si>
+  <si>
+    <t>SAN-080818-01</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>Liked when speaker smiled; asked for copy of results</t>
+  </si>
+  <si>
+    <t>SAN-081018-01</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Eye tracker was fine during calibration but seemed to have some trouble later in experiment</t>
   </si>
 </sst>
 </file>
@@ -241,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,6 +306,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF424242"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -316,6 +347,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +665,7 @@
   <dimension ref="A1:O128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,40 +685,40 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -694,19 +726,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>43301</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
@@ -715,34 +747,34 @@
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>43301</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>0</v>
@@ -751,34 +783,34 @@
         <v>2</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>43301</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -787,34 +819,34 @@
         <v>3</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>43306</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>0</v>
@@ -823,34 +855,34 @@
         <v>1</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>43306</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -859,32 +891,32 @@
         <v>2</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
         <v>43306</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
@@ -893,32 +925,32 @@
         <v>3</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>43306</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -927,32 +959,32 @@
         <v>4</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
         <v>43308</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
@@ -961,34 +993,34 @@
         <v>1</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2">
         <v>43308</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>0</v>
@@ -997,34 +1029,34 @@
         <v>2</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
         <v>43308</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>0</v>
@@ -1033,32 +1065,32 @@
         <v>3</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2">
         <v>43313</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>0</v>
@@ -1067,32 +1099,32 @@
         <v>4</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2">
         <v>43313</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>0</v>
@@ -1101,32 +1133,32 @@
         <v>1</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2">
         <v>43313</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>0</v>
@@ -1135,34 +1167,34 @@
         <v>2</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2">
         <v>43313</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>0</v>
@@ -1171,32 +1203,32 @@
         <v>3</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C16" s="2">
         <v>43315</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>0</v>
@@ -1205,32 +1237,32 @@
         <v>4</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2">
         <v>43315</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>0</v>
@@ -1238,63 +1270,133 @@
       <c r="G17" s="1">
         <v>3</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="H17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43318</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43320</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43322</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
added adult data and restructured data directory
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/elizabeth_adult_subject_log.xlsx
+++ b/data/01_participant_logs/elizabeth_adult_subject_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC_NOVEL/adult_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBCB0D7-4DD5-A842-8B21-E571B6E8AF39}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E62753C-2FFE-6F4E-A35B-819E3213DF03}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{7F77447E-73EC-4A43-A6DE-AF98E6954F7E}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="74">
   <si>
     <t>ES</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>pilot A</t>
   </si>
   <si>
@@ -228,10 +225,28 @@
     <t>NA</t>
   </si>
   <si>
+    <t>SAN-080318-02</t>
+  </si>
+  <si>
     <t>NF</t>
   </si>
   <si>
-    <t>SAN-080318-02</t>
+    <t>SAN-080618-01</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>Wore glasses but eye tracker seemed mostly fine</t>
+  </si>
+  <si>
+    <t>SAN-080818-01</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>Liked when speaker smiled; asked for copy of results</t>
   </si>
 </sst>
 </file>
@@ -241,7 +256,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,6 +297,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF424242"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -316,6 +338,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC254625-20F3-5F48-8577-779CC79D2BAC}">
   <dimension ref="A1:O128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,40 +676,40 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -694,19 +717,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>43301</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
@@ -715,34 +738,36 @@
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>43301</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>0</v>
@@ -751,34 +776,36 @@
         <v>2</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>43301</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -787,34 +814,36 @@
         <v>3</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>43306</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>0</v>
@@ -823,34 +852,36 @@
         <v>1</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>43306</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -859,32 +890,34 @@
         <v>2</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
         <v>43306</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
@@ -893,32 +926,34 @@
         <v>3</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>43306</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -927,32 +962,34 @@
         <v>4</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
         <v>43308</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
@@ -961,34 +998,36 @@
         <v>1</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2">
         <v>43308</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>0</v>
@@ -997,34 +1036,36 @@
         <v>2</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
         <v>43308</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>0</v>
@@ -1033,32 +1074,34 @@
         <v>3</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K11" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2">
         <v>43313</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>0</v>
@@ -1067,32 +1110,34 @@
         <v>4</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2">
         <v>43313</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>0</v>
@@ -1101,32 +1146,34 @@
         <v>1</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2">
         <v>43313</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>0</v>
@@ -1135,34 +1182,36 @@
         <v>2</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2">
         <v>43313</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>0</v>
@@ -1171,32 +1220,34 @@
         <v>3</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C16" s="2">
         <v>43315</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>0</v>
@@ -1205,20 +1256,22 @@
         <v>4</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>67</v>
@@ -1227,10 +1280,10 @@
         <v>43315</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>0</v>
@@ -1238,47 +1291,95 @@
       <c r="G17" s="1">
         <v>3</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="H17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43318</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43320</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>

</xml_diff>